<commit_message>
"Woody Plant,Ground Cover and Forest Mgmt Analysis"
</commit_message>
<xml_diff>
--- a/Understanding Data/Metadata - Edem.xlsx
+++ b/Understanding Data/Metadata - Edem.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Comprehensive Species Tally</t>
   </si>
@@ -104,7 +104,13 @@
     <t>Vikash, Edem, Harwinder</t>
   </si>
   <si>
-    <t>Git test</t>
+    <t>Woody plants info - A more detail explanation is provided in the Understanding data - Edem markdown document</t>
+  </si>
+  <si>
+    <t>Ground cover plants info - A more detail explanation is provided in the Understanding data - Edem markdown document</t>
+  </si>
+  <si>
+    <t>Forest management effort info -  A more detail explanation is provided in the Understanding data - Edem markdown document</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -179,6 +185,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -463,7 +472,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +529,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -531,7 +540,7 @@
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -548,7 +557,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
@@ -559,7 +568,9 @@
       <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -572,7 +583,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -585,7 +596,9 @@
       <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>

</xml_diff>